<commit_message>
Full hmda transmittal join
</commit_message>
<xml_diff>
--- a/Rick_project_schema.xlsx
+++ b/Rick_project_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aki/dev/Rick_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206D9A0B-C9DF-FA47-ADC2-9D9B22731588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC113655-A07D-3243-A584-6649D19E8F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="500" windowWidth="37320" windowHeight="20020" xr2:uid="{7B44C53F-3E20-954E-9CE5-A7A86C00A06C}"/>
+    <workbookView xWindow="1760" yWindow="2060" windowWidth="29980" windowHeight="10140" xr2:uid="{7B44C53F-3E20-954E-9CE5-A7A86C00A06C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="233">
   <si>
     <t>Database tables</t>
   </si>
@@ -1158,7 +1158,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A6E42C0-0994-2249-8A49-4F522E251ABA}">
   <dimension ref="A1:AS154"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="O2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1342,7 +1344,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" ref="D6:D41" si="0">LOWER(P5)</f>
+        <f t="shared" ref="D6:D8" si="0">LOWER(P5)</f>
         <v>acq_branches</v>
       </c>
       <c r="G6" t="s">
@@ -1468,7 +1470,7 @@
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D11" t="str">
-        <f>LOWER(P14)</f>
+        <f t="shared" ref="D11:D42" si="1">LOWER(P14)</f>
         <v>acq_class</v>
       </c>
       <c r="G11" s="13" t="s">
@@ -1483,7 +1485,7 @@
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D12" t="str">
-        <f>LOWER(P15)</f>
+        <f t="shared" si="1"/>
         <v>acq_class_type</v>
       </c>
       <c r="G12" s="11" t="s">
@@ -1552,7 +1554,7 @@
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D13" t="str">
-        <f>LOWER(P16)</f>
+        <f t="shared" si="1"/>
         <v>acq_class_type_desc</v>
       </c>
       <c r="J13" s="2"/>
@@ -1628,7 +1630,7 @@
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D14" t="str">
-        <f>LOWER(P17)</f>
+        <f t="shared" si="1"/>
         <v>acq_clcode</v>
       </c>
       <c r="J14" t="s">
@@ -1709,7 +1711,7 @@
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D15" t="str">
-        <f>LOWER(P18)</f>
+        <f t="shared" si="1"/>
         <v>acq_cntyname</v>
       </c>
       <c r="J15" t="s">
@@ -1790,7 +1792,7 @@
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D16" t="str">
-        <f>LOWER(P19)</f>
+        <f t="shared" si="1"/>
         <v>acq_cntynum</v>
       </c>
       <c r="P16" t="s">
@@ -1868,7 +1870,7 @@
     </row>
     <row r="17" spans="4:44" x14ac:dyDescent="0.2">
       <c r="D17" t="str">
-        <f>LOWER(P20)</f>
+        <f t="shared" si="1"/>
         <v>acq_fdicregion</v>
       </c>
       <c r="P17" t="s">
@@ -1946,7 +1948,7 @@
     </row>
     <row r="18" spans="4:44" x14ac:dyDescent="0.2">
       <c r="D18" t="str">
-        <f>LOWER(P21)</f>
+        <f t="shared" si="1"/>
         <v>acq_fdicregion_desc</v>
       </c>
       <c r="G18" t="s">
@@ -2027,7 +2029,7 @@
     </row>
     <row r="19" spans="4:44" x14ac:dyDescent="0.2">
       <c r="D19" t="str">
-        <f>LOWER(P22)</f>
+        <f t="shared" si="1"/>
         <v>acq_insagent1</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -2111,7 +2113,7 @@
     </row>
     <row r="20" spans="4:44" x14ac:dyDescent="0.2">
       <c r="D20" t="str">
-        <f>LOWER(P23)</f>
+        <f t="shared" si="1"/>
         <v>acq_insagent2</v>
       </c>
       <c r="G20" t="s">
@@ -2129,7 +2131,7 @@
     </row>
     <row r="21" spans="4:44" x14ac:dyDescent="0.2">
       <c r="D21" s="12" t="str">
-        <f>LOWER(P24)</f>
+        <f t="shared" si="1"/>
         <v>acq_instname</v>
       </c>
       <c r="G21" s="11" t="s">
@@ -2147,7 +2149,7 @@
     </row>
     <row r="22" spans="4:44" x14ac:dyDescent="0.2">
       <c r="D22" t="str">
-        <f>LOWER(P25)</f>
+        <f t="shared" si="1"/>
         <v>acq_latitude</v>
       </c>
       <c r="G22" s="11" t="s">
@@ -2220,7 +2222,7 @@
     </row>
     <row r="23" spans="4:44" x14ac:dyDescent="0.2">
       <c r="D23" t="str">
-        <f>LOWER(P26)</f>
+        <f t="shared" si="1"/>
         <v>acq_longitude</v>
       </c>
       <c r="G23" t="s">
@@ -2295,7 +2297,7 @@
     </row>
     <row r="24" spans="4:44" x14ac:dyDescent="0.2">
       <c r="D24" t="str">
-        <f>LOWER(P27)</f>
+        <f t="shared" si="1"/>
         <v>acq_orgtype_num</v>
       </c>
       <c r="G24" s="12" t="s">
@@ -2313,7 +2315,7 @@
     </row>
     <row r="25" spans="4:44" x14ac:dyDescent="0.2">
       <c r="D25" t="str">
-        <f>LOWER(P28)</f>
+        <f t="shared" si="1"/>
         <v>acq_org_eff_dte</v>
       </c>
       <c r="G25" t="s">
@@ -2331,7 +2333,7 @@
     </row>
     <row r="26" spans="4:44" x14ac:dyDescent="0.2">
       <c r="D26" t="str">
-        <f>LOWER(P29)</f>
+        <f t="shared" si="1"/>
         <v>acq_paddr</v>
       </c>
       <c r="G26" s="12" t="s">
@@ -2405,7 +2407,7 @@
     </row>
     <row r="27" spans="4:44" x14ac:dyDescent="0.2">
       <c r="D27" s="12" t="str">
-        <f>LOWER(P30)</f>
+        <f t="shared" si="1"/>
         <v>acq_pcity</v>
       </c>
       <c r="G27" s="12" t="s">
@@ -2480,7 +2482,7 @@
     </row>
     <row r="28" spans="4:44" x14ac:dyDescent="0.2">
       <c r="D28" s="12" t="str">
-        <f>LOWER(P31)</f>
+        <f t="shared" si="1"/>
         <v>acq_pstalp</v>
       </c>
       <c r="G28" s="12" t="s">
@@ -2555,7 +2557,7 @@
     </row>
     <row r="29" spans="4:44" x14ac:dyDescent="0.2">
       <c r="D29" t="str">
-        <f>LOWER(P32)</f>
+        <f t="shared" si="1"/>
         <v>acq_pstnum</v>
       </c>
       <c r="G29" t="s">
@@ -2570,10 +2572,67 @@
       <c r="P29" t="s">
         <v>48</v>
       </c>
+      <c r="U29">
+        <v>2020</v>
+      </c>
+      <c r="V29" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="W29" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="X29" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y29" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z29" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="AA29" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="AB29" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="AC29" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="AD29" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="AE29" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="AF29" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="AG29" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH29" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="AI29" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="AJ29" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="AK29" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="AL29" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="AM29" s="6" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="30" spans="4:44" x14ac:dyDescent="0.2">
       <c r="D30" s="12" t="str">
-        <f>LOWER(P33)</f>
+        <f t="shared" si="1"/>
         <v>acq_pzip5</v>
       </c>
       <c r="G30" t="s">
@@ -2585,7 +2644,7 @@
     </row>
     <row r="31" spans="4:44" x14ac:dyDescent="0.2">
       <c r="D31" t="str">
-        <f>LOWER(P34)</f>
+        <f t="shared" si="1"/>
         <v>acq_pziprest</v>
       </c>
       <c r="G31" t="s">
@@ -2597,7 +2656,7 @@
     </row>
     <row r="32" spans="4:44" x14ac:dyDescent="0.2">
       <c r="D32" t="str">
-        <f>LOWER(P35)</f>
+        <f t="shared" si="1"/>
         <v>acq_regagent</v>
       </c>
       <c r="G32" t="s">
@@ -2609,7 +2668,7 @@
     </row>
     <row r="33" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D33" t="str">
-        <f>LOWER(P36)</f>
+        <f t="shared" si="1"/>
         <v>acq_trust</v>
       </c>
       <c r="G33" t="s">
@@ -2621,7 +2680,7 @@
     </row>
     <row r="34" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D34" t="str">
-        <f>LOWER(P37)</f>
+        <f t="shared" si="1"/>
         <v>acq_uninum</v>
       </c>
       <c r="G34" t="s">
@@ -2633,7 +2692,7 @@
     </row>
     <row r="35" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D35" t="str">
-        <f>LOWER(P38)</f>
+        <f t="shared" si="1"/>
         <v>assisted_payout_flag</v>
       </c>
       <c r="G35" t="s">
@@ -2645,7 +2704,7 @@
     </row>
     <row r="36" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D36" t="str">
-        <f>LOWER(P39)</f>
+        <f t="shared" si="1"/>
         <v>bank_insured</v>
       </c>
       <c r="G36" t="s">
@@ -2657,7 +2716,7 @@
     </row>
     <row r="37" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D37" t="str">
-        <f>LOWER(P40)</f>
+        <f t="shared" si="1"/>
         <v>cert</v>
       </c>
       <c r="G37" t="s">
@@ -2669,7 +2728,7 @@
     </row>
     <row r="38" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D38" t="str">
-        <f>LOWER(P41)</f>
+        <f t="shared" si="1"/>
         <v>changecode</v>
       </c>
       <c r="P38" t="s">
@@ -2678,7 +2737,7 @@
     </row>
     <row r="39" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D39" t="str">
-        <f>LOWER(P42)</f>
+        <f t="shared" si="1"/>
         <v>changecode_desc</v>
       </c>
       <c r="P39" t="s">
@@ -2687,7 +2746,7 @@
     </row>
     <row r="40" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D40" t="str">
-        <f>LOWER(P43)</f>
+        <f t="shared" si="1"/>
         <v>changecode_desc_long</v>
       </c>
       <c r="P40" t="s">
@@ -2696,7 +2755,7 @@
     </row>
     <row r="41" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D41" t="str">
-        <f>LOWER(P44)</f>
+        <f t="shared" si="1"/>
         <v>charter_com_to_other_flag</v>
       </c>
       <c r="P41" t="s">
@@ -2705,7 +2764,7 @@
     </row>
     <row r="42" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D42" t="str">
-        <f>LOWER(P45)</f>
+        <f t="shared" si="1"/>
         <v>charter_com_to_ots_flag</v>
       </c>
       <c r="P42" t="s">
@@ -2714,7 +2773,7 @@
     </row>
     <row r="43" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D43" t="str">
-        <f>LOWER(P46)</f>
+        <f t="shared" ref="D43:D74" si="2">LOWER(P46)</f>
         <v>charter_other_to_com_flag</v>
       </c>
       <c r="P43" t="s">
@@ -2723,7 +2782,7 @@
     </row>
     <row r="44" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D44" t="str">
-        <f>LOWER(P47)</f>
+        <f t="shared" si="2"/>
         <v>charter_ots_to_com_flag</v>
       </c>
       <c r="P44" t="s">
@@ -2732,7 +2791,7 @@
     </row>
     <row r="45" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D45" t="str">
-        <f>LOWER(P48)</f>
+        <f t="shared" si="2"/>
         <v>class</v>
       </c>
       <c r="P45" t="s">
@@ -2741,7 +2800,7 @@
     </row>
     <row r="46" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D46" t="str">
-        <f>LOWER(P49)</f>
+        <f t="shared" si="2"/>
         <v>class_change_flag</v>
       </c>
       <c r="P46" t="s">
@@ -2750,7 +2809,7 @@
     </row>
     <row r="47" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D47" t="str">
-        <f>LOWER(P50)</f>
+        <f t="shared" si="2"/>
         <v>class_type</v>
       </c>
       <c r="P47" t="s">
@@ -2759,7 +2818,7 @@
     </row>
     <row r="48" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D48" t="str">
-        <f>LOWER(P51)</f>
+        <f t="shared" si="2"/>
         <v>class_type_desc</v>
       </c>
       <c r="P48" t="s">
@@ -2768,7 +2827,7 @@
     </row>
     <row r="49" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D49" t="str">
-        <f>LOWER(P52)</f>
+        <f t="shared" si="2"/>
         <v>effdate</v>
       </c>
       <c r="P49" t="s">
@@ -2777,7 +2836,7 @@
     </row>
     <row r="50" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D50" t="str">
-        <f>LOWER(P53)</f>
+        <f t="shared" si="2"/>
         <v>effyear</v>
       </c>
       <c r="P50" t="s">
@@ -2786,7 +2845,7 @@
     </row>
     <row r="51" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D51" t="str">
-        <f>LOWER(P54)</f>
+        <f t="shared" si="2"/>
         <v>enddate</v>
       </c>
       <c r="P51" t="s">
@@ -2795,7 +2854,7 @@
     </row>
     <row r="52" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D52" t="str">
-        <f>LOWER(P55)</f>
+        <f t="shared" si="2"/>
         <v>endyear</v>
       </c>
       <c r="P52" t="s">
@@ -2804,7 +2863,7 @@
     </row>
     <row r="53" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D53" t="str">
-        <f>LOWER(P56)</f>
+        <f t="shared" si="2"/>
         <v>failed_com_to_com_flag</v>
       </c>
       <c r="P53" t="s">
@@ -2813,7 +2872,7 @@
     </row>
     <row r="54" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D54" t="str">
-        <f>LOWER(P57)</f>
+        <f t="shared" si="2"/>
         <v>failed_other_to_com_flag</v>
       </c>
       <c r="P54" t="s">
@@ -2822,7 +2881,7 @@
     </row>
     <row r="55" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D55" t="str">
-        <f>LOWER(P58)</f>
+        <f t="shared" si="2"/>
         <v>failed_ots_to_com_flag</v>
       </c>
       <c r="P55" t="s">
@@ -2831,7 +2890,7 @@
     </row>
     <row r="56" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D56" t="str">
-        <f>LOWER(P59)</f>
+        <f t="shared" si="2"/>
         <v>failed_ots_to_ots_flag</v>
       </c>
       <c r="P56" t="s">
@@ -2840,7 +2899,7 @@
     </row>
     <row r="57" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D57" t="str">
-        <f>LOWER(P60)</f>
+        <f t="shared" si="2"/>
         <v>failed_rtc_flag</v>
       </c>
       <c r="P57" t="s">
@@ -2849,7 +2908,7 @@
     </row>
     <row r="58" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D58" t="str">
-        <f>LOWER(P61)</f>
+        <f t="shared" si="2"/>
         <v>frm_class</v>
       </c>
       <c r="P58" t="s">
@@ -2858,7 +2917,7 @@
     </row>
     <row r="59" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D59" t="str">
-        <f>LOWER(P62)</f>
+        <f t="shared" si="2"/>
         <v>frm_class_type</v>
       </c>
       <c r="P59" t="s">
@@ -2867,7 +2926,7 @@
     </row>
     <row r="60" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D60" t="str">
-        <f>LOWER(P63)</f>
+        <f t="shared" si="2"/>
         <v>frm_class_type_desc</v>
       </c>
       <c r="P60" t="s">
@@ -2876,7 +2935,7 @@
     </row>
     <row r="61" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D61" t="str">
-        <f>LOWER(P64)</f>
+        <f t="shared" si="2"/>
         <v>frm_insagent1</v>
       </c>
       <c r="P61" t="s">
@@ -2885,7 +2944,7 @@
     </row>
     <row r="62" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D62" t="str">
-        <f>LOWER(P65)</f>
+        <f t="shared" si="2"/>
         <v>frm_latitude</v>
       </c>
       <c r="P62" t="s">
@@ -2894,7 +2953,7 @@
     </row>
     <row r="63" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D63" t="str">
-        <f>LOWER(P66)</f>
+        <f t="shared" si="2"/>
         <v>frm_longitude</v>
       </c>
       <c r="P63" t="s">
@@ -2903,7 +2962,7 @@
     </row>
     <row r="64" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D64" t="str">
-        <f>LOWER(P67)</f>
+        <f t="shared" si="2"/>
         <v>frm_orgtype_num</v>
       </c>
       <c r="P64" t="s">
@@ -2912,7 +2971,7 @@
     </row>
     <row r="65" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D65" t="str">
-        <f>LOWER(P68)</f>
+        <f t="shared" si="2"/>
         <v>frm_pstalp</v>
       </c>
       <c r="P65" t="s">
@@ -2921,7 +2980,7 @@
     </row>
     <row r="66" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D66" t="str">
-        <f>LOWER(P69)</f>
+        <f t="shared" si="2"/>
         <v>frm_pstnum</v>
       </c>
       <c r="P66" t="s">
@@ -2930,7 +2989,7 @@
     </row>
     <row r="67" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D67" t="str">
-        <f>LOWER(P70)</f>
+        <f t="shared" si="2"/>
         <v>frm_regagent</v>
       </c>
       <c r="P67" t="s">
@@ -2939,7 +2998,7 @@
     </row>
     <row r="68" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D68" t="str">
-        <f>LOWER(P71)</f>
+        <f t="shared" si="2"/>
         <v>id</v>
       </c>
       <c r="P68" t="s">
@@ -2948,7 +3007,7 @@
     </row>
     <row r="69" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D69" t="str">
-        <f>LOWER(P72)</f>
+        <f t="shared" si="2"/>
         <v>insagent1</v>
       </c>
       <c r="P69" t="s">
@@ -2957,7 +3016,7 @@
     </row>
     <row r="70" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D70" t="str">
-        <f>LOWER(P73)</f>
+        <f t="shared" si="2"/>
         <v>insagent1_change_flag</v>
       </c>
       <c r="P70" t="s">
@@ -2966,7 +3025,7 @@
     </row>
     <row r="71" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D71" t="str">
-        <f>LOWER(P74)</f>
+        <f t="shared" si="2"/>
         <v>insured_com_flag</v>
       </c>
       <c r="P71" t="s">
@@ -2975,7 +3034,7 @@
     </row>
     <row r="72" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D72" t="str">
-        <f>LOWER(P75)</f>
+        <f t="shared" si="2"/>
         <v>insured_ots_flag</v>
       </c>
       <c r="P72" t="s">
@@ -2984,7 +3043,7 @@
     </row>
     <row r="73" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D73" t="str">
-        <f>LOWER(P76)</f>
+        <f t="shared" si="2"/>
         <v>new_charter_denovo_flag</v>
       </c>
       <c r="P73" t="s">
@@ -2993,7 +3052,7 @@
     </row>
     <row r="74" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D74" t="str">
-        <f>LOWER(P77)</f>
+        <f t="shared" si="2"/>
         <v>new_charter_flag</v>
       </c>
       <c r="P74" t="s">
@@ -3002,7 +3061,7 @@
     </row>
     <row r="75" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D75" t="str">
-        <f>LOWER(P78)</f>
+        <f t="shared" ref="D75:D106" si="3">LOWER(P78)</f>
         <v>orgtype_num</v>
       </c>
       <c r="P75" t="s">
@@ -3011,7 +3070,7 @@
     </row>
     <row r="76" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D76" t="str">
-        <f>LOWER(P79)</f>
+        <f t="shared" si="3"/>
         <v>org_role_cde</v>
       </c>
       <c r="P76" t="s">
@@ -3020,7 +3079,7 @@
     </row>
     <row r="77" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D77" t="str">
-        <f>LOWER(P80)</f>
+        <f t="shared" si="3"/>
         <v>org_stat_flg</v>
       </c>
       <c r="P77" t="s">
@@ -3029,7 +3088,7 @@
     </row>
     <row r="78" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D78" t="str">
-        <f>LOWER(P81)</f>
+        <f t="shared" si="3"/>
         <v>out_cert</v>
       </c>
       <c r="P78" t="s">
@@ -3038,7 +3097,7 @@
     </row>
     <row r="79" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D79" t="str">
-        <f>LOWER(P82)</f>
+        <f t="shared" si="3"/>
         <v>out_chartagent</v>
       </c>
       <c r="P79" t="s">
@@ -3047,7 +3106,7 @@
     </row>
     <row r="80" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D80" t="str">
-        <f>LOWER(P83)</f>
+        <f t="shared" si="3"/>
         <v>out_charter</v>
       </c>
       <c r="P80" t="s">
@@ -3056,7 +3115,7 @@
     </row>
     <row r="81" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D81" t="str">
-        <f>LOWER(P84)</f>
+        <f t="shared" si="3"/>
         <v>out_class</v>
       </c>
       <c r="P81" t="s">
@@ -3065,7 +3124,7 @@
     </row>
     <row r="82" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D82" t="str">
-        <f>LOWER(P85)</f>
+        <f t="shared" si="3"/>
         <v>out_class_type</v>
       </c>
       <c r="P82" t="s">
@@ -3074,7 +3133,7 @@
     </row>
     <row r="83" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D83" t="str">
-        <f>LOWER(P86)</f>
+        <f t="shared" si="3"/>
         <v>out_class_type_desc</v>
       </c>
       <c r="P83" t="s">
@@ -3083,7 +3142,7 @@
     </row>
     <row r="84" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D84" t="str">
-        <f>LOWER(P87)</f>
+        <f t="shared" si="3"/>
         <v>out_clcode</v>
       </c>
       <c r="P84" t="s">
@@ -3092,7 +3151,7 @@
     </row>
     <row r="85" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D85" t="str">
-        <f>LOWER(P88)</f>
+        <f t="shared" si="3"/>
         <v>out_cntyname</v>
       </c>
       <c r="P85" t="s">
@@ -3101,7 +3160,7 @@
     </row>
     <row r="86" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D86" t="str">
-        <f>LOWER(P89)</f>
+        <f t="shared" si="3"/>
         <v>out_cntynum</v>
       </c>
       <c r="P86" t="s">
@@ -3110,7 +3169,7 @@
     </row>
     <row r="87" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D87" t="str">
-        <f>LOWER(P90)</f>
+        <f t="shared" si="3"/>
         <v>out_fdicregion</v>
       </c>
       <c r="P87" t="s">
@@ -3119,7 +3178,7 @@
     </row>
     <row r="88" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D88" t="str">
-        <f>LOWER(P91)</f>
+        <f t="shared" si="3"/>
         <v>out_fdicregion_desc</v>
       </c>
       <c r="P88" t="s">
@@ -3128,7 +3187,7 @@
     </row>
     <row r="89" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D89" t="str">
-        <f>LOWER(P92)</f>
+        <f t="shared" si="3"/>
         <v>out_insagent1</v>
       </c>
       <c r="P89" t="s">
@@ -3137,7 +3196,7 @@
     </row>
     <row r="90" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D90" t="str">
-        <f>LOWER(P93)</f>
+        <f t="shared" si="3"/>
         <v>out_insagent2</v>
       </c>
       <c r="P90" t="s">
@@ -3146,7 +3205,7 @@
     </row>
     <row r="91" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D91" t="str">
-        <f>LOWER(P94)</f>
+        <f t="shared" si="3"/>
         <v>out_instname</v>
       </c>
       <c r="P91" t="s">
@@ -3155,7 +3214,7 @@
     </row>
     <row r="92" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D92" t="str">
-        <f>LOWER(P95)</f>
+        <f t="shared" si="3"/>
         <v>out_latitude</v>
       </c>
       <c r="P92" t="s">
@@ -3164,7 +3223,7 @@
     </row>
     <row r="93" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D93" t="str">
-        <f>LOWER(P96)</f>
+        <f t="shared" si="3"/>
         <v>out_longitude</v>
       </c>
       <c r="P93" t="s">
@@ -3173,7 +3232,7 @@
     </row>
     <row r="94" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D94" t="str">
-        <f>LOWER(P97)</f>
+        <f t="shared" si="3"/>
         <v>out_orgtype_num</v>
       </c>
       <c r="P94" t="s">
@@ -3182,7 +3241,7 @@
     </row>
     <row r="95" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D95" t="str">
-        <f>LOWER(P98)</f>
+        <f t="shared" si="3"/>
         <v>out_paddr</v>
       </c>
       <c r="P95" t="s">
@@ -3191,7 +3250,7 @@
     </row>
     <row r="96" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D96" t="str">
-        <f>LOWER(P99)</f>
+        <f t="shared" si="3"/>
         <v>out_pcity</v>
       </c>
       <c r="P96" t="s">
@@ -3200,7 +3259,7 @@
     </row>
     <row r="97" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D97" t="str">
-        <f>LOWER(P100)</f>
+        <f t="shared" si="3"/>
         <v>out_pstalp</v>
       </c>
       <c r="P97" t="s">
@@ -3209,7 +3268,7 @@
     </row>
     <row r="98" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D98" t="str">
-        <f>LOWER(P101)</f>
+        <f t="shared" si="3"/>
         <v>out_pstnum</v>
       </c>
       <c r="P98" t="s">
@@ -3218,7 +3277,7 @@
     </row>
     <row r="99" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D99" t="str">
-        <f>LOWER(P102)</f>
+        <f t="shared" si="3"/>
         <v>out_pzip5</v>
       </c>
       <c r="P99" t="s">
@@ -3227,7 +3286,7 @@
     </row>
     <row r="100" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D100" t="str">
-        <f>LOWER(P103)</f>
+        <f t="shared" si="3"/>
         <v>out_pziprest</v>
       </c>
       <c r="P100" t="s">
@@ -3236,7 +3295,7 @@
     </row>
     <row r="101" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D101" t="str">
-        <f>LOWER(P104)</f>
+        <f t="shared" si="3"/>
         <v>out_regagent</v>
       </c>
       <c r="P101" t="s">
@@ -3245,7 +3304,7 @@
     </row>
     <row r="102" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D102" t="str">
-        <f>LOWER(P105)</f>
+        <f t="shared" si="3"/>
         <v>out_trust</v>
       </c>
       <c r="P102" t="s">
@@ -3254,7 +3313,7 @@
     </row>
     <row r="103" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D103" t="str">
-        <f>LOWER(P106)</f>
+        <f t="shared" si="3"/>
         <v>out_uninum</v>
       </c>
       <c r="P103" t="s">
@@ -3263,7 +3322,7 @@
     </row>
     <row r="104" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D104" t="str">
-        <f>LOWER(P107)</f>
+        <f t="shared" si="3"/>
         <v>procdate</v>
       </c>
       <c r="P104" t="s">
@@ -3272,7 +3331,7 @@
     </row>
     <row r="105" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D105" t="str">
-        <f>LOWER(P108)</f>
+        <f t="shared" si="3"/>
         <v>procyear</v>
       </c>
       <c r="P105" t="s">
@@ -3281,7 +3340,7 @@
     </row>
     <row r="106" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D106" t="str">
-        <f>LOWER(P109)</f>
+        <f t="shared" si="3"/>
         <v>pstalp</v>
       </c>
       <c r="P106" t="s">
@@ -3290,7 +3349,7 @@
     </row>
     <row r="107" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D107" t="str">
-        <f>LOWER(P110)</f>
+        <f t="shared" ref="D107:D138" si="4">LOWER(P110)</f>
         <v>regagent</v>
       </c>
       <c r="P107" t="s">
@@ -3299,7 +3358,7 @@
     </row>
     <row r="108" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D108" t="str">
-        <f>LOWER(P111)</f>
+        <f t="shared" si="4"/>
         <v>regagent_change_flag</v>
       </c>
       <c r="P108" t="s">
@@ -3308,7 +3367,7 @@
     </row>
     <row r="109" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D109" t="str">
-        <f>LOWER(P112)</f>
+        <f t="shared" si="4"/>
         <v>relocate_flag</v>
       </c>
       <c r="P109" t="s">
@@ -3317,7 +3376,7 @@
     </row>
     <row r="110" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D110" t="str">
-        <f>LOWER(P113)</f>
+        <f t="shared" si="4"/>
         <v>report_type</v>
       </c>
       <c r="P110" t="s">
@@ -3326,7 +3385,7 @@
     </row>
     <row r="111" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D111" t="str">
-        <f>LOWER(P114)</f>
+        <f t="shared" si="4"/>
         <v>stnum</v>
       </c>
       <c r="P111" t="s">
@@ -3335,7 +3394,7 @@
     </row>
     <row r="112" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D112" t="str">
-        <f>LOWER(P115)</f>
+        <f t="shared" si="4"/>
         <v>sur_cert</v>
       </c>
       <c r="P112" t="s">
@@ -3344,7 +3403,7 @@
     </row>
     <row r="113" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D113" t="str">
-        <f>LOWER(P116)</f>
+        <f t="shared" si="4"/>
         <v>sur_changecode</v>
       </c>
       <c r="P113" t="s">
@@ -3353,7 +3412,7 @@
     </row>
     <row r="114" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D114" t="str">
-        <f>LOWER(P117)</f>
+        <f t="shared" si="4"/>
         <v>sur_changecode_desc</v>
       </c>
       <c r="P114" t="s">
@@ -3362,7 +3421,7 @@
     </row>
     <row r="115" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D115" t="str">
-        <f>LOWER(P118)</f>
+        <f t="shared" si="4"/>
         <v>sur_chartagent</v>
       </c>
       <c r="P115" t="s">
@@ -3371,7 +3430,7 @@
     </row>
     <row r="116" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D116" t="str">
-        <f>LOWER(P119)</f>
+        <f t="shared" si="4"/>
         <v>sur_charter</v>
       </c>
       <c r="P116" t="s">
@@ -3380,7 +3439,7 @@
     </row>
     <row r="117" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D117" t="str">
-        <f>LOWER(P120)</f>
+        <f t="shared" si="4"/>
         <v>sur_class_type</v>
       </c>
       <c r="P117" t="s">
@@ -3389,7 +3448,7 @@
     </row>
     <row r="118" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D118" t="str">
-        <f>LOWER(P121)</f>
+        <f t="shared" si="4"/>
         <v>sur_class_type_desc</v>
       </c>
       <c r="P118" t="s">
@@ -3398,7 +3457,7 @@
     </row>
     <row r="119" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D119" t="str">
-        <f>LOWER(P122)</f>
+        <f t="shared" si="4"/>
         <v>sur_clcode</v>
       </c>
       <c r="P119" t="s">
@@ -3410,7 +3469,7 @@
     </row>
     <row r="120" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D120" t="str">
-        <f>LOWER(P123)</f>
+        <f t="shared" si="4"/>
         <v>sur_cntyname</v>
       </c>
       <c r="P120" t="s">
@@ -3419,7 +3478,7 @@
     </row>
     <row r="121" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D121" t="str">
-        <f>LOWER(P124)</f>
+        <f t="shared" si="4"/>
         <v>sur_cntynum</v>
       </c>
       <c r="P121" t="s">
@@ -3428,7 +3487,7 @@
     </row>
     <row r="122" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D122" t="str">
-        <f>LOWER(P125)</f>
+        <f t="shared" si="4"/>
         <v>sur_fdicregion</v>
       </c>
       <c r="P122" t="s">
@@ -3437,7 +3496,7 @@
     </row>
     <row r="123" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D123" t="str">
-        <f>LOWER(P126)</f>
+        <f t="shared" si="4"/>
         <v>sur_fdicregion_desc</v>
       </c>
       <c r="P123" t="s">
@@ -3446,7 +3505,7 @@
     </row>
     <row r="124" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D124" t="str">
-        <f>LOWER(P127)</f>
+        <f t="shared" si="4"/>
         <v>sur_insagent1</v>
       </c>
       <c r="P124" t="s">
@@ -3455,7 +3514,7 @@
     </row>
     <row r="125" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D125" t="str">
-        <f>LOWER(P128)</f>
+        <f t="shared" si="4"/>
         <v>sur_insagent2</v>
       </c>
       <c r="P125" t="s">
@@ -3464,7 +3523,7 @@
     </row>
     <row r="126" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D126" t="str">
-        <f>LOWER(P129)</f>
+        <f t="shared" si="4"/>
         <v>sur_instname</v>
       </c>
       <c r="P126" t="s">
@@ -3473,7 +3532,7 @@
     </row>
     <row r="127" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D127" t="str">
-        <f>LOWER(P130)</f>
+        <f t="shared" si="4"/>
         <v>sur_latitude</v>
       </c>
       <c r="P127" t="s">
@@ -3482,7 +3541,7 @@
     </row>
     <row r="128" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D128" t="str">
-        <f>LOWER(P131)</f>
+        <f t="shared" si="4"/>
         <v>sur_longitude</v>
       </c>
       <c r="P128" t="s">
@@ -3491,7 +3550,7 @@
     </row>
     <row r="129" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D129" t="str">
-        <f>LOWER(P132)</f>
+        <f t="shared" si="4"/>
         <v>sur_maddr</v>
       </c>
       <c r="P129" t="s">
@@ -3500,7 +3559,7 @@
     </row>
     <row r="130" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D130" t="str">
-        <f>LOWER(P133)</f>
+        <f t="shared" si="4"/>
         <v>sur_mcity</v>
       </c>
       <c r="P130" t="s">
@@ -3509,7 +3568,7 @@
     </row>
     <row r="131" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D131" t="str">
-        <f>LOWER(P134)</f>
+        <f t="shared" si="4"/>
         <v>sur_mstalp</v>
       </c>
       <c r="P131" t="s">
@@ -3518,7 +3577,7 @@
     </row>
     <row r="132" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D132" t="str">
-        <f>LOWER(P135)</f>
+        <f t="shared" si="4"/>
         <v>sur_mstate</v>
       </c>
       <c r="P132" t="s">
@@ -3527,7 +3586,7 @@
     </row>
     <row r="133" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D133" t="str">
-        <f>LOWER(P136)</f>
+        <f t="shared" si="4"/>
         <v>sur_mzip5</v>
       </c>
       <c r="P133" t="s">
@@ -3536,7 +3595,7 @@
     </row>
     <row r="134" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D134" t="str">
-        <f>LOWER(P137)</f>
+        <f t="shared" si="4"/>
         <v>sur_orgtype_num</v>
       </c>
       <c r="P134" t="s">
@@ -3545,7 +3604,7 @@
     </row>
     <row r="135" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D135" t="str">
-        <f>LOWER(P138)</f>
+        <f t="shared" si="4"/>
         <v>sur_paddr</v>
       </c>
       <c r="P135" t="s">
@@ -3554,7 +3613,7 @@
     </row>
     <row r="136" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D136" t="str">
-        <f>LOWER(P139)</f>
+        <f t="shared" si="4"/>
         <v>sur_pcity</v>
       </c>
       <c r="P136" t="s">
@@ -3563,7 +3622,7 @@
     </row>
     <row r="137" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D137" t="str">
-        <f>LOWER(P140)</f>
+        <f t="shared" si="4"/>
         <v>sur_pstalp</v>
       </c>
       <c r="P137" t="s">
@@ -3572,7 +3631,7 @@
     </row>
     <row r="138" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D138" t="str">
-        <f>LOWER(P141)</f>
+        <f t="shared" si="4"/>
         <v>sur_pstnum</v>
       </c>
       <c r="P138" t="s">
@@ -3581,7 +3640,7 @@
     </row>
     <row r="139" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D139" t="str">
-        <f>LOWER(P142)</f>
+        <f t="shared" ref="D139:D170" si="5">LOWER(P142)</f>
         <v>sur_pzip5</v>
       </c>
       <c r="P139" t="s">
@@ -3590,7 +3649,7 @@
     </row>
     <row r="140" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D140" t="str">
-        <f>LOWER(P143)</f>
+        <f t="shared" si="5"/>
         <v>sur_pziprest</v>
       </c>
       <c r="P140" t="s">
@@ -3599,7 +3658,7 @@
     </row>
     <row r="141" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D141" t="str">
-        <f>LOWER(P144)</f>
+        <f t="shared" si="5"/>
         <v>sur_regagent</v>
       </c>
       <c r="P141" t="s">
@@ -3608,7 +3667,7 @@
     </row>
     <row r="142" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D142" t="str">
-        <f>LOWER(P145)</f>
+        <f t="shared" si="5"/>
         <v>sur_trust</v>
       </c>
       <c r="P142" t="s">
@@ -3617,7 +3676,7 @@
     </row>
     <row r="143" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D143" t="str">
-        <f>LOWER(P146)</f>
+        <f t="shared" si="5"/>
         <v>transnum</v>
       </c>
       <c r="P143" t="s">
@@ -3626,7 +3685,7 @@
     </row>
     <row r="144" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D144" t="str">
-        <f>LOWER(P147)</f>
+        <f t="shared" si="5"/>
         <v>unassist_com_to_com_flag</v>
       </c>
       <c r="P144" t="s">
@@ -3635,7 +3694,7 @@
     </row>
     <row r="145" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D145" t="str">
-        <f>LOWER(P148)</f>
+        <f t="shared" si="5"/>
         <v>unassist_com_to_ots_flag</v>
       </c>
       <c r="P145" t="s">
@@ -3644,7 +3703,7 @@
     </row>
     <row r="146" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D146" t="str">
-        <f>LOWER(P149)</f>
+        <f t="shared" si="5"/>
         <v>unassist_other_to_com_flag</v>
       </c>
       <c r="P146" t="s">
@@ -3653,7 +3712,7 @@
     </row>
     <row r="147" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D147" t="str">
-        <f>LOWER(P150)</f>
+        <f t="shared" si="5"/>
         <v>unassist_ots_to_com_flag</v>
       </c>
       <c r="P147" t="s">
@@ -3662,7 +3721,7 @@
     </row>
     <row r="148" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D148" t="str">
-        <f>LOWER(P151)</f>
+        <f t="shared" si="5"/>
         <v>unassist_ots_to_ots_flag</v>
       </c>
       <c r="P148" t="s">
@@ -3671,7 +3730,7 @@
     </row>
     <row r="149" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D149" t="str">
-        <f>LOWER(P152)</f>
+        <f t="shared" si="5"/>
         <v>uninum</v>
       </c>
       <c r="P149" t="s">
@@ -3680,7 +3739,7 @@
     </row>
     <row r="150" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D150" t="str">
-        <f>LOWER(P153)</f>
+        <f t="shared" si="5"/>
         <v>voluntary_liquidation_flag</v>
       </c>
       <c r="P150" t="s">
@@ -3689,7 +3748,7 @@
     </row>
     <row r="151" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D151" t="str">
-        <f>LOWER(P154)</f>
+        <f t="shared" si="5"/>
         <v>withdraw_insurance_com_flag</v>
       </c>
       <c r="P151" t="s">

</xml_diff>